<commit_message>
Kostenplan und Angebot angepasst.
</commit_message>
<xml_diff>
--- a/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
+++ b/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Documents/GitHub/ITP-Project-1/Abgabe/Projekt Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8118A471-44AB-4D48-9EEA-57E9A01F921B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3FF31C-85E9-1E45-BBF2-0B1E885B3029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00874EB8-F1B6-C647-8C3A-93D1CC03828B}"/>
+    <workbookView xWindow="17720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00874EB8-F1B6-C647-8C3A-93D1CC03828B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Geplante Kalkulation der Kosten</t>
   </si>
@@ -86,9 +86,6 @@
     <t xml:space="preserve">Vertriebskosten </t>
   </si>
   <si>
-    <t>Notizen</t>
-  </si>
-  <si>
     <t>Serverkosten</t>
   </si>
   <si>
@@ -125,18 +122,12 @@
     <t>Instandhaltung</t>
   </si>
   <si>
-    <t>beinhaltet die Anschaffung und Wartung von Computern, Monitoren, Software und anderer technologischer Ausrüstung, die für die Entwicklung des Spiels erforderlich sind.</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
     <t>Dauer:</t>
   </si>
   <si>
-    <t>Putzkraft</t>
-  </si>
-  <si>
     <t>inkl. Gewinn:</t>
   </si>
   <si>
@@ -150,6 +141,45 @@
   </si>
   <si>
     <t>Projekt managment  (36 / Stunde)</t>
+  </si>
+  <si>
+    <t>Gewinn:</t>
+  </si>
+  <si>
+    <t>Prozentualer Anteil</t>
+  </si>
+  <si>
+    <t>Geld</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Kosten Entwicklung</t>
+  </si>
+  <si>
+    <t>Kosten Marketing</t>
+  </si>
+  <si>
+    <t>Kunden Kosten Aufstellung</t>
+  </si>
+  <si>
+    <t>Maintainance</t>
+  </si>
+  <si>
+    <t>Split 1</t>
+  </si>
+  <si>
+    <t>Split 2</t>
+  </si>
+  <si>
+    <t>Netto</t>
+  </si>
+  <si>
+    <t>Brutto</t>
+  </si>
+  <si>
+    <t>USt.</t>
   </si>
 </sst>
 </file>
@@ -159,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +227,11 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -213,12 +248,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -306,49 +341,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,21 +364,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -398,8 +382,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
@@ -713,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF95868-752C-3C48-A399-C404830A1278}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,543 +734,703 @@
     <col min="2" max="2" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="161.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>C7*C6</f>
+        <v>1597.6695</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5">
-        <f>SUM(E10:E15,E17,E19:E22,E24:E27,E29:E31)</f>
+      <c r="C7" s="5">
+        <f>SUM(E12:E17,E19,E21:E24,E26:E29,E31:E33)</f>
         <v>15976.695</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="6">
-        <f>C6*115%</f>
-        <v>18373.199249999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="6">
+        <f>C7+D6</f>
+        <v>17574.3645</v>
+      </c>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="G10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
+      <c r="G11" s="31">
+        <f>SUM(E12:E17) / C7</f>
+        <v>5.5874822671397303E-2</v>
+      </c>
+      <c r="H11" s="34">
+        <f>E7*G11</f>
+        <v>981.96449999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <f>11/10</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C12" s="10">
         <f xml:space="preserve"> 780 / 2</f>
         <v>390</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11">
-        <f>C10*D10</f>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <f>C12*D12</f>
         <v>390</v>
       </c>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="G12" s="32"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <f>12/10</f>
         <v>1.2</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10">
         <f xml:space="preserve"> 212.91 / 2</f>
         <v>106.455</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11">
-        <f t="shared" ref="E11:E15" si="0">C11*D11</f>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" ref="E13:E17" si="0">C13*D13</f>
         <v>106.455</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="G13" s="32"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <f>13/10</f>
         <v>1.3</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="10">
         <f xml:space="preserve"> 150 / 2</f>
         <v>75</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="G14" s="32"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <f>14/10</f>
         <v>1.4</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="10">
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="10">
         <v>49.95</v>
       </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11">
         <f t="shared" si="0"/>
         <v>49.95</v>
       </c>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="G15" s="32"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <f>15/10</f>
         <v>1.5</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="10">
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10">
         <v>21.29</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
         <f t="shared" si="0"/>
         <v>21.29</v>
       </c>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="G16" s="32"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <f>16/10</f>
         <v>1.6</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="10">
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10">
         <f xml:space="preserve"> 500 / 2</f>
         <v>250</v>
       </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="G17" s="32"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="G18" s="31">
+        <f>SUM(E19) / C7</f>
+        <v>4.1184988509826347E-2</v>
+      </c>
+      <c r="H18" s="34">
+        <f>G18*E7</f>
+        <v>723.80000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <f>21/10</f>
         <v>2.1</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C19" s="10">
         <v>329</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D19" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="11">
-        <f>C17*D17</f>
+      <c r="E19" s="11">
+        <f>C19*D19</f>
         <v>658</v>
       </c>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="G19" s="32"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="G20" s="31">
+        <f>SUM(E21:E23) / C7</f>
+        <v>0.67323060244938016</v>
+      </c>
+      <c r="H20" s="34">
+        <f>G20*E7</f>
+        <v>11831.599999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <f>31/10</f>
         <v>3.1</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10">
         <v>2880</v>
       </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="11">
-        <f>C19*D19</f>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="11">
+        <f>C21*D21</f>
         <v>2880</v>
       </c>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="G21" s="32"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <f>32/10</f>
         <v>3.2</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="10">
         <f>7500 / 2</f>
         <v>3750</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="11">
-        <f t="shared" ref="E20:E22" si="1">C20*D20</f>
+      <c r="E22" s="11">
+        <f t="shared" ref="E22:E24" si="1">C22*D22</f>
         <v>7500</v>
       </c>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="G22" s="32"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <f>33/10</f>
         <v>3.3</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="10">
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="10">
         <v>376</v>
       </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="11">
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
         <f t="shared" si="1"/>
         <v>376</v>
       </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="G23" s="32"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <f>34/10</f>
         <v>3.4</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="10">
         <f xml:space="preserve"> 1700 / 2</f>
         <v>850</v>
       </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="11">
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11">
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="G24" s="32">
+        <f>SUM(E24) / C7</f>
+        <v>5.3202492755854702E-2</v>
+      </c>
+      <c r="H24" s="36">
+        <f>G24*E7</f>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>4</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B25" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
+      <c r="G25" s="31">
+        <f>SUM(E26:E29) / C7</f>
+        <v>0.10484020631300779</v>
+      </c>
+      <c r="H25" s="34">
+        <f>G25*E7</f>
+        <v>1842.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <f>41/10</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C24" s="10">
-        <f xml:space="preserve"> 400 / 2</f>
-        <v>200</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="11">
-        <f>C24*D24</f>
-        <v>400</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <f>42/10</f>
-        <v>4.2</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="10">
-        <f xml:space="preserve"> 800 / 2</f>
-        <v>400</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="11">
-        <f t="shared" ref="E25:E27" si="2">C25*D25</f>
-        <v>800</v>
-      </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <f>43/10</f>
-        <v>4.3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C26" s="10">
         <f xml:space="preserve"> 400 / 2</f>
         <v>200</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="11">
+        <f>C26*D26</f>
+        <v>400</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f>42/10</f>
+        <v>4.2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="10">
+        <f xml:space="preserve"> 800 / 2</f>
+        <v>400</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" ref="E27:E29" si="2">C27*D27</f>
+        <v>800</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f>43/10</f>
+        <v>4.3</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="10">
+        <f xml:space="preserve"> 400 / 2</f>
+        <v>200</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="11">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="G28" s="32"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <f>44/10</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="10">
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="10">
         <f xml:space="preserve"> 550 / 2</f>
         <v>275</v>
       </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11">
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11">
         <f t="shared" si="2"/>
         <v>275</v>
       </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="G29" s="32"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B30" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="G30" s="31">
+        <f>SUM(E31:E33) / C7</f>
+        <v>7.166688730053368E-2</v>
+      </c>
+      <c r="H30" s="34">
+        <f>G30*E7</f>
+        <v>1259.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <f>51/10</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C31" s="10">
         <v>30</v>
       </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="11">
-        <f>C29*D29</f>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="11">
+        <f>C31*D31</f>
         <v>30</v>
       </c>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="G31" s="32"/>
+      <c r="H31" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <f>52/10</f>
         <v>5.2</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="10">
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="10">
         <v>1100</v>
       </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="11">
-        <f t="shared" ref="E30:E31" si="3">C30*D30</f>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" ref="E32:E33" si="3">C32*D32</f>
         <v>1100</v>
       </c>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
+      <c r="G32" s="32"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="12">
         <f>53/10</f>
         <v>5.3</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="14">
+      <c r="B33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="14">
         <v>15</v>
       </c>
-      <c r="D31" s="13">
-        <v>1</v>
-      </c>
-      <c r="E31" s="15">
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+      <c r="E33" s="15">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="G34" s="26">
+        <f>SUM(G11:G33)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="35">
+        <f>SUM(H11:H33)</f>
+        <v>17574.364499999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="35">
+        <f>H20+H25</f>
+        <v>13674.099999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="35">
+        <f>H24+H18+H11</f>
+        <v>2640.7645000000002</v>
+      </c>
+      <c r="D37" s="35">
+        <f>C37*70%</f>
+        <v>1848.5351499999999</v>
+      </c>
+      <c r="E37" s="35">
+        <f>C37*30%</f>
+        <v>792.22935000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="35">
+        <f>H30</f>
+        <v>1259.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="35">
+        <f>C36+D37+E37+C38</f>
+        <v>17574.364499999996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="35">
+        <f>C39*19%</f>
+        <v>3339.1292549999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="35">
+        <f>C39+C40</f>
+        <v>20913.493754999996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed UML and made Graphical Changes to Kostenplan
</commit_message>
<xml_diff>
--- a/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
+++ b/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Documents/GitHub/ITP-Project-1/Abgabe/Projekt Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3FF31C-85E9-1E45-BBF2-0B1E885B3029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FFC7E8-0E11-6B43-BEC9-63DBC770A524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00874EB8-F1B6-C647-8C3A-93D1CC03828B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00874EB8-F1B6-C647-8C3A-93D1CC03828B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -173,13 +173,13 @@
     <t>Split 2</t>
   </si>
   <si>
-    <t>Netto</t>
-  </si>
-  <si>
-    <t>Brutto</t>
-  </si>
-  <si>
     <t>USt.</t>
+  </si>
+  <si>
+    <t>Summe Netto</t>
+  </si>
+  <si>
+    <t>Summe Brutto</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,12 +211,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Roboto"/>
@@ -232,6 +226,23 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -242,13 +253,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FF0E0E14"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,65 +358,71 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -414,6 +431,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0E0E14"/>
+      <color rgb="FF78BE20"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -423,6 +446,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6513</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>20321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>423253</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6524803C-686C-D089-186F-497FC9E2E258}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="362113" y="20321"/>
+          <a:ext cx="416740" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF95868-752C-3C48-A399-C404830A1278}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,20 +813,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -765,29 +837,29 @@
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="17">
         <v>0.1</v>
       </c>
       <c r="D6" s="5">
@@ -811,7 +883,7 @@
         <f>C7+D6</f>
         <v>17574.3645</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E8" s="4"/>
@@ -836,10 +908,10 @@
       <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -847,17 +919,17 @@
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="G11" s="31">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="G11" s="37">
         <f>SUM(E12:E17) / C7</f>
         <v>5.5874822671397303E-2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="38">
         <f>E7*G11</f>
         <v>981.96449999999993</v>
       </c>
@@ -881,7 +953,7 @@
         <f>C12*D12</f>
         <v>390</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -903,7 +975,7 @@
         <f t="shared" ref="E13:E17" si="0">C13*D13</f>
         <v>106.455</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -925,7 +997,7 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G14" s="32"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -946,7 +1018,7 @@
         <f t="shared" si="0"/>
         <v>49.95</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -967,7 +1039,7 @@
         <f t="shared" si="0"/>
         <v>21.29</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -989,24 +1061,24 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="G18" s="31">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+      <c r="G18" s="37">
         <f>SUM(E19) / C7</f>
         <v>4.1184988509826347E-2</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="38">
         <f>G18*E7</f>
         <v>723.80000000000007</v>
       </c>
@@ -1029,24 +1101,24 @@
         <f>C19*D19</f>
         <v>658</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-      <c r="G20" s="31">
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+      <c r="G20" s="37">
         <f>SUM(E21:E23) / C7</f>
         <v>0.67323060244938016</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="38">
         <f>G20*E7</f>
         <v>11831.599999999999</v>
       </c>
@@ -1069,7 +1141,7 @@
         <f>C21*D21</f>
         <v>2880</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1091,7 +1163,7 @@
         <f t="shared" ref="E22:E24" si="1">C22*D22</f>
         <v>7500</v>
       </c>
-      <c r="G22" s="32"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1112,7 +1184,7 @@
         <f t="shared" si="1"/>
         <v>376</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1134,11 +1206,11 @@
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="21">
         <f>SUM(E24) / C7</f>
         <v>5.3202492755854702E-2</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="24">
         <f>G24*E7</f>
         <v>935</v>
       </c>
@@ -1147,17 +1219,17 @@
       <c r="A25" s="3">
         <v>4</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
-      <c r="G25" s="31">
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
+      <c r="G25" s="37">
         <f>SUM(E26:E29) / C7</f>
         <v>0.10484020631300779</v>
       </c>
-      <c r="H25" s="34">
+      <c r="H25" s="38">
         <f>G25*E7</f>
         <v>1842.5</v>
       </c>
@@ -1181,7 +1253,7 @@
         <f>C26*D26</f>
         <v>400</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="21"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1203,7 +1275,7 @@
         <f t="shared" ref="E27:E29" si="2">C27*D27</f>
         <v>800</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="21"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1225,7 +1297,7 @@
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="21"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1247,24 +1319,24 @@
         <f t="shared" si="2"/>
         <v>275</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="21"/>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>5</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
-      <c r="G30" s="31">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
+      <c r="G30" s="37">
         <f>SUM(E31:E33) / C7</f>
         <v>7.166688730053368E-2</v>
       </c>
-      <c r="H30" s="34">
+      <c r="H30" s="38">
         <f>G30*E7</f>
         <v>1259.5</v>
       </c>
@@ -1287,7 +1359,7 @@
         <f>C31*D31</f>
         <v>30</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="4" t="s">
         <v>38</v>
       </c>
@@ -1310,7 +1382,7 @@
         <f t="shared" ref="E32:E33" si="3">C32*D32</f>
         <v>1100</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="21"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1331,96 +1403,96 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="30"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="G34" s="26">
-        <f>SUM(G11:G33)</f>
-        <v>1</v>
-      </c>
-      <c r="H34" s="35">
-        <f>SUM(H11:H33)</f>
-        <v>17574.364499999996</v>
-      </c>
+      <c r="G34" s="16"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="41" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="23">
         <f>H20+H25</f>
         <v>13674.099999999999</v>
       </c>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="35">
+      <c r="C37" s="23">
         <f>H24+H18+H11</f>
         <v>2640.7645000000002</v>
       </c>
-      <c r="D37" s="35">
+      <c r="D37" s="23">
         <f>C37*70%</f>
         <v>1848.5351499999999</v>
       </c>
-      <c r="E37" s="35">
+      <c r="E37" s="24">
         <f>C37*30%</f>
         <v>792.22935000000007</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="23">
         <f>H30</f>
         <v>1259.5</v>
       </c>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="35">
+      <c r="B39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="23">
         <f>C36+D37+E37+C38</f>
         <v>17574.364499999996</v>
       </c>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="35">
+      <c r="B40" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="23">
         <f>C39*19%</f>
         <v>3339.1292549999994</v>
       </c>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="35">
+      <c r="B41" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="43">
         <f>C39+C40</f>
         <v>20913.493754999996</v>
       </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1434,5 +1506,9 @@
     <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C27" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replay Viewer i think? idk tbh
</commit_message>
<xml_diff>
--- a/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
+++ b/Abgabe/Projekt Dokumentation/Kostenplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Documents/GitHub/ITP-Project-1/Abgabe/Projekt Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC268BC-9DCD-AF4B-955A-0961B3070BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09130BF-3965-3347-B441-9DF0868DDC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00874EB8-F1B6-C647-8C3A-93D1CC03828B}"/>
   </bookViews>
@@ -134,24 +134,12 @@
     <t>Pong - Multiplayer</t>
   </si>
   <si>
-    <t>2 Wochen ( etwa 80 Stunden)</t>
-  </si>
-  <si>
-    <t>Entwickler (46,88 / Stunde)</t>
-  </si>
-  <si>
-    <t>Projekt managment  (36 / Stunde)</t>
-  </si>
-  <si>
     <t>Gewinn:</t>
   </si>
   <si>
     <t>Prozentualer Anteil</t>
   </si>
   <si>
-    <t>Geld</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -180,13 +168,26 @@
   </si>
   <si>
     <t>Summe Brutto</t>
+  </si>
+  <si>
+    <t>Teilkosten</t>
+  </si>
+  <si>
+    <t>Stunden</t>
+  </si>
+  <si>
+    <t>Entwickler (76,88 / Stunde)</t>
+  </si>
+  <si>
+    <t>Projekt managment  (65 / Stunde)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
@@ -358,7 +359,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,6 +394,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,6 +430,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
@@ -796,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF95868-752C-3C48-A399-C404830A1278}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -813,20 +821,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -837,34 +845,36 @@
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
+      <c r="C5" s="34">
+        <v>80</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="17">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="5">
         <f>C7*C6</f>
-        <v>1597.6695</v>
+        <v>4266.415</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -874,14 +884,14 @@
       </c>
       <c r="C7" s="5">
         <f>SUM(E12:E17,E19,E21:E24,E26:E29,E31:E33)</f>
-        <v>15976.695</v>
+        <v>21332.075000000001</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="6">
         <f>C7+D6</f>
-        <v>17574.3645</v>
+        <v>25598.49</v>
       </c>
       <c r="G7" s="23"/>
     </row>
@@ -909,29 +919,29 @@
         <v>10</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
       <c r="G11" s="27">
         <f>SUM(E12:E17) / C7</f>
-        <v>5.5874822671397303E-2</v>
+        <v>4.0177760485091106E-2</v>
       </c>
       <c r="H11" s="28">
         <f>E7*G11</f>
-        <v>981.96449999999993</v>
+        <v>1028.4899999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -943,7 +953,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10">
-        <f xml:space="preserve"> 780 / 2</f>
+        <f xml:space="preserve"> 780 / 160 *C5</f>
         <v>390</v>
       </c>
       <c r="D12" s="1">
@@ -965,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="10">
-        <f xml:space="preserve"> 212.91 / 2</f>
+        <f xml:space="preserve"> 212.91 / 160 *C5</f>
         <v>106.455</v>
       </c>
       <c r="D13" s="1">
@@ -987,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="10">
-        <f xml:space="preserve"> 150 / 2</f>
+        <f xml:space="preserve"> 150/ 160 *C5</f>
         <v>75</v>
       </c>
       <c r="D14" s="1">
@@ -1009,14 +1019,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="10">
-        <v>49.95</v>
+        <f>49.95 / 160 *C5</f>
+        <v>24.975000000000001</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>49.95</v>
+        <v>24.975000000000001</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="4"/>
@@ -1030,14 +1041,15 @@
         <v>26</v>
       </c>
       <c r="C16" s="10">
-        <v>21.29</v>
+        <f xml:space="preserve"> 21.29 / 160 *C5</f>
+        <v>10.645</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>21.29</v>
+        <v>10.645</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="4"/>
@@ -1051,7 +1063,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="10">
-        <f xml:space="preserve"> 500 / 2</f>
+        <f xml:space="preserve"> 500 / 160 *C5</f>
         <v>250</v>
       </c>
       <c r="D17" s="1">
@@ -1068,19 +1080,19 @@
       <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
       <c r="G18" s="27">
         <f>SUM(E19) / C7</f>
-        <v>4.1184988509826347E-2</v>
+        <v>1.5422784703316483E-2</v>
       </c>
       <c r="H18" s="28">
         <f>G18*E7</f>
-        <v>723.80000000000007</v>
+        <v>394.8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1092,14 +1104,15 @@
         <v>12</v>
       </c>
       <c r="C19" s="10">
-        <v>329</v>
+        <f xml:space="preserve"> 329 / 160 *C5</f>
+        <v>164.5</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="11">
         <f>C19*D19</f>
-        <v>658</v>
+        <v>329</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="4"/>
@@ -1108,19 +1121,19 @@
       <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
       <c r="G20" s="27">
         <f>SUM(E21:E23) / C7</f>
-        <v>0.67323060244938016</v>
+        <v>0.77235805705727167</v>
       </c>
       <c r="H20" s="28">
         <f>G20*E7</f>
-        <v>11831.599999999999</v>
+        <v>19771.2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1129,17 +1142,17 @@
         <v>3.1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C21" s="10">
-        <v>2880</v>
+        <v>5200</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="11">
         <f>C21*D21</f>
-        <v>2880</v>
+        <v>5200</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="4"/>
@@ -1150,18 +1163,17 @@
         <v>3.2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C22" s="10">
-        <f>7500 / 2</f>
-        <v>3750</v>
+        <v>5450</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" ref="E22:E24" si="1">C22*D22</f>
-        <v>7500</v>
+        <v>10900</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="4"/>
@@ -1208,30 +1220,30 @@
       </c>
       <c r="G24" s="21">
         <f>SUM(E24) / C7</f>
-        <v>5.3202492755854702E-2</v>
+        <v>3.9846100297322225E-2</v>
       </c>
       <c r="H24" s="24">
         <f>G24*E7</f>
-        <v>935</v>
+        <v>1020.0000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>4</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43"/>
       <c r="G25" s="27">
         <f>SUM(E26:E29) / C7</f>
-        <v>0.10484020631300779</v>
+        <v>7.8520256468252614E-2</v>
       </c>
       <c r="H25" s="28">
         <f>G25*E7</f>
-        <v>1842.5</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1326,19 +1338,19 @@
       <c r="A30" s="3">
         <v>5</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
       <c r="G30" s="27">
         <f>SUM(E31:E33) / C7</f>
-        <v>7.166688730053368E-2</v>
+        <v>5.3675040988745822E-2</v>
       </c>
       <c r="H30" s="28">
         <f>G30*E7</f>
-        <v>1259.5</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1361,7 +1373,7 @@
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1414,88 +1426,87 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C36" s="23">
         <f>H20+H25</f>
-        <v>13674.099999999999</v>
+        <v>21781.200000000001</v>
       </c>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37" s="23">
         <f>H24+H18+H11</f>
-        <v>2640.7645000000002</v>
+        <v>2443.29</v>
       </c>
       <c r="D37" s="23">
         <f>C37*70%</f>
-        <v>1848.5351499999999</v>
+        <v>1710.3029999999999</v>
       </c>
       <c r="E37" s="24">
         <f>C37*30%</f>
-        <v>792.22935000000007</v>
+        <v>732.98699999999997</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" s="26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C38" s="23">
         <f>H30</f>
-        <v>1259.5</v>
+        <v>1374</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C39" s="23">
         <f>C36+D37+E37+C38</f>
-        <v>17574.364499999996</v>
+        <v>25598.49</v>
       </c>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="23">
-        <f>C39*19%</f>
-        <v>3339.1292549999994</v>
+        <v>41</v>
+      </c>
+      <c r="C40" s="46">
+        <v>4863.71</v>
       </c>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C41" s="33">
         <f>C39+C40</f>
-        <v>20913.493754999996</v>
+        <v>30462.2</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="C4:E4"/>
@@ -1503,7 +1514,6 @@
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>